<commit_message>
cleaning up lm models for cali
</commit_message>
<xml_diff>
--- a/data/fisheries/participation/cmck_laa.xlsx
+++ b/data/fisheries/participation/cmck_laa.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Export" sheetId="1" r:id="Rca50dab3ffa4489a"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Export" sheetId="1" r:id="R4eb99adb00d842a8"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -12,7 +12,6 @@
   <x:numFmts>
     <x:numFmt numFmtId="181" formatCode="0"/>
     <x:numFmt numFmtId="182" formatCode="#,0"/>
-    <x:numFmt numFmtId="183" formatCode="\$#,0;(\$#,0);\$#,0"/>
   </x:numFmts>
   <x:fonts>
     <x:font/>
@@ -52,9 +51,7 @@
     </x:xf>
     <x:xf numFmtId="181"/>
     <x:xf numFmtId="182"/>
-    <x:xf numFmtId="183"/>
     <x:xf numFmtId="182" fontId="1"/>
-    <x:xf numFmtId="183" fontId="1"/>
   </x:cellXfs>
 </x:styleSheet>
 </file>
@@ -75,7 +72,7 @@
       </x:c>
       <x:c s="2" t="inlineStr">
         <x:is>
-          <x:t>Value</x:t>
+          <x:t>Participation</x:t>
         </x:is>
       </x:c>
     </x:row>
@@ -86,8 +83,8 @@
       <x:c s="9">
         <x:v>50582515.25</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>4417984.115</x:v>
+      <x:c s="9">
+        <x:v>107</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -97,8 +94,8 @@
       <x:c s="9">
         <x:v>63972204.599999994</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>6002496.1715</x:v>
+      <x:c s="9">
+        <x:v>120</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -108,8 +105,8 @@
       <x:c s="9">
         <x:v>32940473.43</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>2893905.9531</x:v>
+      <x:c s="9">
+        <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -119,8 +116,8 @@
       <x:c s="9">
         <x:v>32280459</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>2800173.105</x:v>
+      <x:c s="9">
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -130,8 +127,8 @@
       <x:c s="9">
         <x:v>3976477</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>336903.52</x:v>
+      <x:c s="9">
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -141,8 +138,8 @@
       <x:c s="9">
         <x:v>36144511</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>2567142.135</x:v>
+      <x:c s="9">
+        <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -152,8 +149,8 @@
       <x:c s="9">
         <x:v>43794596</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>2636614.39</x:v>
+      <x:c s="9">
+        <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -163,8 +160,8 @@
       <x:c s="9">
         <x:v>55618278.3</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>1715387.357</x:v>
+      <x:c s="9">
+        <x:v>101</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -174,8 +171,8 @@
       <x:c s="9">
         <x:v>65028062.9</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>3670506.994</x:v>
+      <x:c s="9">
+        <x:v>95</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -185,8 +182,8 @@
       <x:c s="9">
         <x:v>45839940.2</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>2671086.531</x:v>
+      <x:c s="9">
+        <x:v>95</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -196,8 +193,8 @@
       <x:c s="9">
         <x:v>63194982.9</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>3372337.33</x:v>
+      <x:c s="9">
+        <x:v>88</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -207,8 +204,8 @@
       <x:c s="9">
         <x:v>69219365.83</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>4970498.455</x:v>
+      <x:c s="9">
+        <x:v>88</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -218,8 +215,8 @@
       <x:c s="9">
         <x:v>39852281.3</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>3541503.06</x:v>
+      <x:c s="9">
+        <x:v>89</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -229,8 +226,8 @@
       <x:c s="9">
         <x:v>25801760.4</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>1392216.783</x:v>
+      <x:c s="9">
+        <x:v>97</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -240,8 +237,8 @@
       <x:c s="9">
         <x:v>21702454.799999997</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>1042941.6615</x:v>
+      <x:c s="9">
+        <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -251,8 +248,8 @@
       <x:c s="9">
         <x:v>17337490.439999998</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>1010281.759</x:v>
+      <x:c s="9">
+        <x:v>92</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -262,8 +259,8 @@
       <x:c s="9">
         <x:v>19318359.6</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>1085274.244</x:v>
+      <x:c s="9">
+        <x:v>97</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -273,8 +270,8 @@
       <x:c s="9">
         <x:v>30868730.450000003</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>2002412.164</x:v>
+      <x:c s="9">
+        <x:v>100</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -284,8 +281,8 @@
       <x:c s="9">
         <x:v>38883343.599999994</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>1790948.473</x:v>
+      <x:c s="9">
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -295,8 +292,8 @@
       <x:c s="9">
         <x:v>18731665.5</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>1035652.5815</x:v>
+      <x:c s="9">
+        <x:v>66</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -306,8 +303,8 @@
       <x:c s="9">
         <x:v>47714707.9</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>2894683.285</x:v>
+      <x:c s="9">
+        <x:v>68</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -317,8 +314,8 @@
       <x:c s="9">
         <x:v>14719022.25</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>1065868.95</x:v>
+      <x:c s="9">
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -328,8 +325,8 @@
       <x:c s="9">
         <x:v>7421269.3</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>486036.1725</x:v>
+      <x:c s="9">
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -339,8 +336,8 @@
       <x:c s="9">
         <x:v>8724804</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>622837.28</x:v>
+      <x:c s="9">
+        <x:v>50</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -350,8 +347,8 @@
       <x:c s="9">
         <x:v>6634637</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>499040.2075</x:v>
+      <x:c s="9">
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -361,8 +358,8 @@
       <x:c s="9">
         <x:v>6934605.8</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>517474.89</x:v>
+      <x:c s="9">
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -372,8 +369,8 @@
       <x:c s="9">
         <x:v>12594563</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>800618.134</x:v>
+      <x:c s="9">
+        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -383,8 +380,8 @@
       <x:c s="9">
         <x:v>10770144.000000002</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>762549.24</x:v>
+      <x:c s="9">
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -394,8 +391,8 @@
       <x:c s="9">
         <x:v>7028372.3</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>633239.03</x:v>
+      <x:c s="9">
+        <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -405,8 +402,8 @@
       <x:c s="9">
         <x:v>11048839.4</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>1083165.817</x:v>
+      <x:c s="9">
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -416,8 +413,8 @@
       <x:c s="9">
         <x:v>4508877.7</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>408731.7035</x:v>
+      <x:c s="9">
+        <x:v>46</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -427,8 +424,8 @@
       <x:c s="9">
         <x:v>2945570.25</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>322459.339</x:v>
+      <x:c s="9">
+        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -438,8 +435,8 @@
       <x:c s="9">
         <x:v>7594964.1999999993</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>871039.25</x:v>
+      <x:c s="9">
+        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -449,8 +446,8 @@
       <x:c s="9">
         <x:v>17792499</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>1517161.7</x:v>
+      <x:c s="9">
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -460,8 +457,8 @@
       <x:c s="9">
         <x:v>11009668</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>1119887.55</x:v>
+      <x:c s="9">
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -471,8 +468,8 @@
       <x:c s="9">
         <x:v>6379512.3999999994</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>688066.48</x:v>
+      <x:c s="9">
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -482,8 +479,8 @@
       <x:c s="9">
         <x:v>3213178</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>393854.035</x:v>
+      <x:c s="9">
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -493,8 +490,8 @@
       <x:c s="9">
         <x:v>4406582</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>577137.655</x:v>
+      <x:c s="9">
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -504,8 +501,8 @@
       <x:c s="9">
         <x:v>4225463</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>754147.274</x:v>
+      <x:c s="9">
+        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -515,8 +512,8 @@
       <x:c s="9">
         <x:v>7940299</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>1236098.217</x:v>
+      <x:c s="9">
+        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -526,8 +523,8 @@
       <x:c s="9">
         <x:v>1198583.2</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>245178.1319</x:v>
+      <x:c s="9">
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -537,8 +534,8 @@
       <x:c s="9">
         <x:v>1884249</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>448933.227</x:v>
+      <x:c s="9">
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -548,8 +545,8 @@
       <x:c s="9">
         <x:v>1124283.73</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>307471.5639</x:v>
+      <x:c s="9">
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -559,8 +556,8 @@
       <x:c s="9">
         <x:v>1107171.1</x:v>
       </x:c>
-      <x:c s="10">
-        <x:v>300002.535</x:v>
+      <x:c s="9">
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -569,11 +566,11 @@
           <x:t>Total</x:t>
         </x:is>
       </x:c>
-      <x:c s="11">
+      <x:c s="10">
         <x:v>984009818.03000009</x:v>
       </x:c>
-      <x:c s="12">
-        <x:v>69511948.4499</x:v>
+      <x:c s="10">
+        <x:v>700</x:v>
       </x:c>
     </x:row>
     <x:row/>

</xml_diff>